<commit_message>
Updated tests for new structure of mu
</commit_message>
<xml_diff>
--- a/tests/testthat/likelihood_calculations.xlsx
+++ b/tests/testthat/likelihood_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Marsden\clustord\tests\testthat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240A23D9-0D41-4974-8CC6-6EC6C67A9894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10ACF153-6E9E-4EF9-806C-7AE07E7A6420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11520" yWindow="120" windowWidth="17280" windowHeight="9060" tabRatio="372" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OSM" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Binary" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -4400,8 +4401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V91"/>
   <sheetViews>
-    <sheetView topLeftCell="H54" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="R97" sqref="R97"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7595,8 +7596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D2DA2D9-F29D-4DBB-9461-1402B0C64181}">
   <dimension ref="A1:AC153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F105" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="I151" sqref="I151"/>
+    <sheetView topLeftCell="A108" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="J157" sqref="J157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>